<commit_message>
add possibility to compare sheets
</commit_message>
<xml_diff>
--- a/test/Excel01.xlsx
+++ b/test/Excel01.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -33,6 +33,9 @@
     <t xml:space="preserve">Success Criteria</t>
   </si>
   <si>
+    <t xml:space="preserve">Creator</t>
+  </si>
+  <si>
     <t xml:space="preserve">TP-01</t>
   </si>
   <si>
@@ -40,6 +43,9 @@
   </si>
   <si>
     <t xml:space="preserve">Komponente ist eingeschaltet Komponente gibt Töne von sich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N.N.</t>
   </si>
   <si>
     <t xml:space="preserve">TP-02</t>
@@ -279,16 +285,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.47"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -301,38 +308,47 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -357,11 +373,11 @@
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -386,25 +402,25 @@
       <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fix; update test files
</commit_message>
<xml_diff>
--- a/test/Excel01.xlsx
+++ b/test/Excel01.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
@@ -82,6 +83,24 @@
   </si>
   <si>
     <t xml:space="preserve">test6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Col1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Col2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Col3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text3</t>
   </si>
 </sst>
 </file>
@@ -287,8 +306,8 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -432,4 +451,50 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>